<commit_message>
after homework1 and lab3
</commit_message>
<xml_diff>
--- a/CSCE206_TA_Status.xlsx
+++ b/CSCE206_TA_Status.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>S:No</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Array index 0 to be counted for even index. The no of files for lab programs.</t>
   </si>
   <si>
-    <t>Cary</t>
-  </si>
-  <si>
     <t>Mode</t>
   </si>
   <si>
@@ -63,6 +60,21 @@
   </si>
   <si>
     <t>01/22/2016</t>
+  </si>
+  <si>
+    <t>KAYLA S REVELLE</t>
+  </si>
+  <si>
+    <t>01/29/2016</t>
+  </si>
+  <si>
+    <t>Lab 2 &amp; Homework 1 questions</t>
+  </si>
+  <si>
+    <t>Lab 1 questions</t>
+  </si>
+  <si>
+    <t>LIN, YU-TING</t>
   </si>
 </sst>
 </file>
@@ -406,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +448,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>4</v>
@@ -456,7 +468,7 @@
         <v>0.55069444444444449</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>7</v>
@@ -467,16 +479,59 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2">
         <v>0.64583333333333337</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>